<commit_message>
#3550 fix typo in trx import sheet
</commit_message>
<xml_diff>
--- a/tpd/template_transactions_order_invoice_payment.xlsx
+++ b/tpd/template_transactions_order_invoice_payment.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23525"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steffenbartsch/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jascha/dev/osapiens/assets/tpd/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{28528B96-6B49-2B4F-941C-8F93E3A54842}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E8727C8A-432B-40BD-9EF8-1797AAE34850}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45048A38-150F-4041-B9EB-ADBB0078B5E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16600" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Order-Import" sheetId="7" r:id="rId1"/>
     <sheet name="Invoice-Import" sheetId="8" r:id="rId2"/>
-    <sheet name="Pament-Import" sheetId="9" r:id="rId3"/>
+    <sheet name="Payment-Import" sheetId="9" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -141,7 +141,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -636,48 +636,48 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -693,7 +693,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -991,21 +991,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93287E3B-03F0-5743-BA61-E7EDE2D3AC73}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="19.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1">
+    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B2" s="5"/>
     </row>
   </sheetData>
@@ -1040,30 +1040,30 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B2" s="5"/>
     </row>
   </sheetData>
@@ -1135,20 +1135,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DE8C40E-08F8-3240-8C2C-F6626D1C6D14}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="10.875" style="6"/>
-    <col min="3" max="17" width="10.875" style="4"/>
-    <col min="18" max="16384" width="10.875" style="6"/>
+    <col min="1" max="2" width="10.83203125" style="6"/>
+    <col min="3" max="17" width="10.83203125" style="4"/>
+    <col min="18" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>21</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="7"/>
     </row>
   </sheetData>
@@ -1217,15 +1217,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101005F4998C67BB1DD4F9504D874A6E091B6" ma:contentTypeVersion="11" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="34481ec151ea5bcde50d4d2ccfc1c21c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="24afc823-56a0-4ca7-beb0-a997ee0e27fa" xmlns:ns3="d1469970-2593-4797-80af-60ba6d9ed68e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="32bbb49a5a99fbcbd9dc86efa7c6a962" ns2:_="" ns3:_="">
     <xsd:import namespace="24afc823-56a0-4ca7-beb0-a997ee0e27fa"/>
@@ -1436,14 +1427,47 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F1768D9-E0D1-4076-A5CD-D313E7369453}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F1768D9-E0D1-4076-A5CD-D313E7369453}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FEBE8E5-297C-4A96-8575-CB8F77254FC3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C07890CA-0447-4E50-AB91-B283364F2404}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="24afc823-56a0-4ca7-beb0-a997ee0e27fa"/>
+    <ds:schemaRef ds:uri="d1469970-2593-4797-80af-60ba6d9ed68e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C07890CA-0447-4E50-AB91-B283364F2404}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FEBE8E5-297C-4A96-8575-CB8F77254FC3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>